<commit_message>
improve tests and cfg
</commit_message>
<xml_diff>
--- a/Lab03_WBT_Form.xlsx
+++ b/Lab03_WBT_Form.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\mures\Desktop\ssvv\LabAssiAsseProjectV03_remastered\LabAssiAsseProjectV03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DAEE602-6973-4439-8858-519AC0014772}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B117792-03AC-4201-9DAB-1963476AB3BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="947" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="947" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem" sheetId="5" r:id="rId1"/>
@@ -23,12 +23,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>No TC</t>
   </si>
@@ -251,12 +251,6 @@
     <t>Save a new assignment</t>
   </si>
   <si>
-    <t>1-2-3-12-E</t>
-  </si>
-  <si>
-    <t>1-2-3-4-5-14-E</t>
-  </si>
-  <si>
     <t>An assignment has: number (unique): integer, brief description: string, deadline: integer (value between 1 and 14), the week it was received: integer (value between 1 and 14).</t>
   </si>
   <si>
@@ -264,12 +258,6 @@
   </si>
   <si>
     <t>R</t>
-  </si>
-  <si>
-    <t>R - ValidatorException if input data is invalid, or repository changed containing the new assignment</t>
-  </si>
-  <si>
-    <t>14-13-E</t>
   </si>
   <si>
     <t>1-2-3-4-5-6-15-13-E</t>
@@ -286,11 +274,17 @@
   <si>
     <t>1-2-3-4-5-6-7-8-18-9-11-E</t>
   </si>
+  <si>
+    <t>R - ValidatorException or NumberFormatException if input data is invalid, or repository changed containing the new assignment</t>
+  </si>
+  <si>
+    <t>1-E</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -836,6 +830,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -843,15 +845,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -868,6 +861,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -905,26 +919,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -954,7 +948,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1508,12 +1502,12 @@
             <a:rPr lang="en-US" sz="1200"/>
             <a:t>){</a:t>
           </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1200"/>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200"/>
-            <a:t>12.	        </a:t>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>	        </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200">
@@ -2432,7 +2426,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2482,78 +2476,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Oval 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13077B7D-7623-4634-AF3B-34D976E9779C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6134100" y="1457325"/>
-          <a:ext cx="742950" cy="676275"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="lt1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000"/>
-            <a:t>1</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1600"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2568,7 +2500,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6143625" y="2343149"/>
+          <a:off x="7334250" y="2133599"/>
           <a:ext cx="742950" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -2606,137 +2538,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Diamond 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A14EF81C-8A97-43A7-9CFE-AC06554BB023}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6096000" y="3381375"/>
-          <a:ext cx="914400" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="lt1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000"/>
-            <a:t>3</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Diamond 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234AF1EB-6F55-46C7-B719-03971AC92FC1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7581900" y="4886324"/>
-          <a:ext cx="914400" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="diamond">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="lt1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000"/>
-            <a:t>5</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2791,13 +2601,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2852,13 +2662,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2911,16 +2721,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2932,14 +2742,15 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="2" idx="4"/>
+          <a:cxnSpLocks/>
+          <a:stCxn id="47" idx="3"/>
           <a:endCxn id="6" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6505575" y="2133600"/>
-          <a:ext cx="9525" cy="209549"/>
+          <a:off x="7019925" y="1476374"/>
+          <a:ext cx="685800" cy="657225"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2967,69 +2778,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180973</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C37ACEB7-F7E4-42DD-996D-9B3B588A8668}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6515100" y="3019424"/>
-          <a:ext cx="38100" cy="361951"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:rowOff>57148</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3042,17 +2800,19 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
-          <a:stCxn id="3" idx="3"/>
+          <a:stCxn id="54" idx="4"/>
           <a:endCxn id="125" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7010400" y="3838575"/>
-          <a:ext cx="361950" cy="476249"/>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="8010525" y="3609973"/>
+          <a:ext cx="66675" cy="447675"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -3078,15 +2838,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3100,16 +2860,19 @@
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
           <a:stCxn id="125" idx="6"/>
-          <a:endCxn id="9" idx="0"/>
+          <a:endCxn id="66" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7743825" y="4652962"/>
-          <a:ext cx="295275" cy="233362"/>
+        <a:xfrm flipH="1">
+          <a:off x="8058150" y="4205287"/>
+          <a:ext cx="581025" cy="709612"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
+        <a:prstGeom prst="bentConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -39344"/>
+            <a:gd name="adj2" fmla="val 73825"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -3135,14 +2898,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3155,14 +2918,15 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="9" idx="3"/>
+          <a:cxnSpLocks/>
+          <a:stCxn id="66" idx="6"/>
           <a:endCxn id="12" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8496300" y="5343524"/>
-          <a:ext cx="314325" cy="285750"/>
+          <a:off x="8429625" y="5253037"/>
+          <a:ext cx="381000" cy="185737"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -3192,13 +2956,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3247,13 +3011,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3303,13 +3067,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3364,13 +3128,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3426,13 +3190,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3486,77 +3250,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="55" name="Oval 54">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F056D02C-5180-4EBD-A3F4-DACBFD59E9AB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5286375" y="4314824"/>
-          <a:ext cx="742950" cy="676275"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="lt1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000"/>
-            <a:t>12</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1600"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3610,77 +3312,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="57" name="Oval 56">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{942CEBCA-C20A-4F8D-94AE-15EF088F1C44}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6934200" y="5886449"/>
-          <a:ext cx="742950" cy="676275"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="lt1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="2000"/>
-            <a:t>14</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1600"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3736,13 +3376,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3798,13 +3438,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3860,13 +3500,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3920,127 +3560,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>123823</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="1026" name="Connector: Elbow 1025">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB862F5C-D191-4A54-9346-659E620F57A6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="3" idx="1"/>
-          <a:endCxn id="55" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="5657850" y="3838574"/>
-          <a:ext cx="438150" cy="476249"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9523</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>171448</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="1030" name="Connector: Elbow 1029">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B3D5EA4-BD55-4060-90E0-C32717773A05}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="9" idx="1"/>
-          <a:endCxn id="57" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="7305676" y="5343523"/>
-          <a:ext cx="276225" cy="542925"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4090,13 +3618,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>304801</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4145,13 +3673,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>161926</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>28573</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>400051</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>114298</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4201,13 +3729,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4257,13 +3785,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>609601</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>85726</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4315,13 +3843,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4371,13 +3899,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>238126</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>38098</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>104776</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>23811</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4427,13 +3955,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>52388</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4481,16 +4009,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142873</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4502,17 +4030,20 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="55" idx="4"/>
+          <a:cxnSpLocks/>
+          <a:stCxn id="47" idx="1"/>
           <a:endCxn id="61" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="3421856" y="7227093"/>
-          <a:ext cx="6491288" cy="2019300"/>
+        <a:xfrm rot="10800000" flipH="1" flipV="1">
+          <a:off x="6105524" y="1476373"/>
+          <a:ext cx="1571625" cy="9815513"/>
         </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -14545"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -4539,13 +4070,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>104773</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>104776</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>52386</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4594,72 +4125,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>342901</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="1053" name="Connector: Elbow 1052">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1ABFB14-A0D7-4BAD-9C8A-07AE99143696}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="57" idx="4"/>
-          <a:endCxn id="56" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="5819776" y="7277099"/>
-          <a:ext cx="2200275" cy="771525"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4708,13 +4181,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>552451</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>66676</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4764,13 +4237,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>552451</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>161926</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4818,16 +4291,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4842,7 +4315,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7000875" y="4314824"/>
+          <a:off x="7896225" y="3867149"/>
           <a:ext cx="742950" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -4882,13 +4355,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4944,13 +4417,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4994,6 +4467,245 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="Diamond 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3932EB72-02FB-4586-8051-D36017FBDF71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6105525" y="1019174"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000"/>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Oval 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22DD9DF5-AE75-48C5-80BF-79A5F35C1642}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7448550" y="3124199"/>
+          <a:ext cx="742950" cy="676275"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000"/>
+            <a:t>3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE9FC296-446A-4AA7-ADAD-B76127D84F98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="4"/>
+          <a:endCxn id="54" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7705725" y="2809874"/>
+          <a:ext cx="114300" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="Oval 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2893721-7DF5-4D9F-ADF1-885922F81FFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7686675" y="4914899"/>
+          <a:ext cx="742950" cy="676275"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000"/>
+            <a:t>5</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5319,11 +5031,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5350,7 +5062,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5358,7 +5070,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5369,7 +5081,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5377,7 +5089,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -5386,11 +5098,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="R3:T16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="R3:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5403,11 +5115,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R3" s="35" t="s">
+      <c r="R3" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="36"/>
-      <c r="T3" s="37"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="45"/>
     </row>
     <row r="4" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R4" s="1" t="s">
@@ -5417,7 +5129,7 @@
         <v>16</v>
       </c>
       <c r="T4" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="18:20" x14ac:dyDescent="0.25">
@@ -5428,7 +5140,7 @@
         <v>13</v>
       </c>
       <c r="T5" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="18:20" x14ac:dyDescent="0.25">
@@ -5439,21 +5151,21 @@
         <v>15</v>
       </c>
       <c r="T6" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R9" s="35" t="s">
+      <c r="R9" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="S9" s="37"/>
+      <c r="S9" s="45"/>
     </row>
     <row r="10" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R10" s="1">
         <v>1</v>
       </c>
       <c r="S10" s="25" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="18:20" x14ac:dyDescent="0.25">
@@ -5461,10 +5173,7 @@
         <v>2</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="18:20" x14ac:dyDescent="0.25">
@@ -5472,7 +5181,7 @@
         <v>3</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="18:20" x14ac:dyDescent="0.25">
@@ -5480,31 +5189,23 @@
         <v>4</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R14" s="1">
         <v>5</v>
       </c>
-      <c r="S14" s="1" t="s">
-        <v>57</v>
+      <c r="S14" s="35" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="18:20" x14ac:dyDescent="0.25">
       <c r="R15" s="1">
         <v>6</v>
       </c>
-      <c r="S15" s="62" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R16" s="1">
-        <v>7</v>
-      </c>
-      <c r="S16" s="62" t="s">
-        <v>59</v>
+      <c r="S15" s="35" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -5519,10 +5220,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:AD19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -5540,26 +5241,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="38" t="s">
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
       <c r="X1" s="24" t="s">
         <v>23</v>
       </c>
@@ -5572,43 +5273,43 @@
     </row>
     <row r="2" spans="2:30" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10"/>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43" t="s">
+      <c r="D2" s="47"/>
+      <c r="E2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="44"/>
+      <c r="F2" s="49"/>
       <c r="G2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="39">
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="52">
         <v>1</v>
       </c>
-      <c r="S2" s="39">
+      <c r="S2" s="52">
         <v>2</v>
       </c>
-      <c r="T2" s="39">
+      <c r="T2" s="52">
         <v>3</v>
       </c>
-      <c r="U2" s="39">
+      <c r="U2" s="52">
         <v>4</v>
       </c>
-      <c r="V2" s="39">
+      <c r="V2" s="52">
         <v>5</v>
       </c>
-      <c r="W2" s="39">
+      <c r="W2" s="52">
         <v>6</v>
       </c>
       <c r="X2" s="24"/>
@@ -5664,12 +5365,12 @@
       <c r="Q3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="40"/>
-      <c r="S3" s="40"/>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
-      <c r="V3" s="40"/>
-      <c r="W3" s="40"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53"/>
       <c r="X3" s="24" t="s">
         <v>24</v>
       </c>
@@ -5891,70 +5592,70 @@
       <c r="AD9" s="26"/>
     </row>
     <row r="10" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B10" s="63">
+      <c r="B10" s="36">
         <v>7</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="67"/>
-      <c r="S10" s="67"/>
-      <c r="T10" s="67"/>
-      <c r="U10" s="67"/>
-      <c r="V10" s="67"/>
-      <c r="W10" s="67"/>
-      <c r="X10" s="68"/>
-      <c r="Y10" s="68"/>
-      <c r="Z10" s="68"/>
-      <c r="AA10" s="69"/>
-      <c r="AB10" s="68"/>
-      <c r="AC10" s="69"/>
-      <c r="AD10" s="69"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="40"/>
+      <c r="W10" s="40"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="41"/>
+      <c r="Z10" s="41"/>
+      <c r="AA10" s="42"/>
+      <c r="AB10" s="41"/>
+      <c r="AC10" s="42"/>
+      <c r="AD10" s="42"/>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B11" s="63">
+      <c r="B11" s="36">
         <v>8</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="67"/>
-      <c r="S11" s="67"/>
-      <c r="T11" s="67"/>
-      <c r="U11" s="67"/>
-      <c r="V11" s="67"/>
-      <c r="W11" s="67"/>
-      <c r="X11" s="68"/>
-      <c r="Y11" s="68"/>
-      <c r="Z11" s="68"/>
-      <c r="AA11" s="69"/>
-      <c r="AB11" s="68"/>
-      <c r="AC11" s="69"/>
-      <c r="AD11" s="69"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="39"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="40"/>
+      <c r="W11" s="40"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="42"/>
+      <c r="AB11" s="41"/>
+      <c r="AC11" s="42"/>
+      <c r="AD11" s="42"/>
     </row>
     <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
@@ -5962,22 +5663,22 @@
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="9" t="s">
@@ -5986,6 +5687,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="C2:D2"/>
@@ -5996,13 +5704,6 @@
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R1:W1"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6010,7 +5711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6024,75 +5725,75 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="54"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="66"/>
       <c r="H4" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="55" t="s">
+      <c r="I4" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
       <c r="M4" s="33"/>
     </row>
     <row r="5" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="56" t="s">
+      <c r="H5" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="46" t="s">
+      <c r="J5" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="46" t="s">
+      <c r="L5" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="49" t="s">
+      <c r="M5" s="61" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="58"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="50"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="62"/>
     </row>
     <row r="7" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="28" t="s">
@@ -6123,11 +5824,6 @@
     <row r="8" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="F5:F6"/>
@@ -6137,6 +5833,11 @@
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>